<commit_message>
udpated Simple LP CSV importer. Multiple publisher separator changes from ',' to ';' , as far as Publisher can have a ',' character in their name
</commit_message>
<xml_diff>
--- a/modules/landlibrary/importers/simple_lp_csv_importer/simple_lp_csv_importer_Mapping.xlsx
+++ b/modules/landlibrary/importers/simple_lp_csv_importer/simple_lp_csv_importer_Mapping.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlos\Documents\projects\data\landlibrary\importers\GLTN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlos\Documents\projects\drupal\modules\landlibrary\importers\simple_lp_csv_importer\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Hoja1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -204,9 +204,6 @@
     <t>importer_gtln_simple_lp_csv</t>
   </si>
   <si>
-    <t>The value of the field must match the organization label.  "," values separator</t>
-  </si>
-  <si>
     <t>Resource types</t>
   </si>
   <si>
@@ -226,6 +223,9 @@
   </si>
   <si>
     <t>Copyright owner</t>
+  </si>
+  <si>
+    <t>The value of the field must match the organization label.  ";" values separator</t>
   </si>
 </sst>
 </file>
@@ -1072,7 +1072,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1137,7 +1137,7 @@
         <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>48</v>
@@ -1187,7 +1187,7 @@
         <v>45</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>44</v>
@@ -1201,7 +1201,7 @@
         <v>46</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>3</v>
@@ -1223,13 +1223,13 @@
         <v>40</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>48</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
@@ -1289,7 +1289,7 @@
         <v>50</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>48</v>
@@ -1303,7 +1303,7 @@
         <v>52</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>48</v>
@@ -1391,7 +1391,7 @@
         <v>33</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
updated simple CSV importer. Now, use ';' as separator in all cases
</commit_message>
<xml_diff>
--- a/modules/landlibrary/importers/simple_lp_csv_importer/simple_lp_csv_importer_Mapping.xlsx
+++ b/modules/landlibrary/importers/simple_lp_csv_importer/simple_lp_csv_importer_Mapping.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Hoja1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="73">
   <si>
     <t>Data provider</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Direct</t>
   </si>
   <si>
-    <t xml:space="preserve">Resource title (field_doc_title) </t>
-  </si>
-  <si>
     <t>Tamper</t>
   </si>
   <si>
@@ -84,9 +81,6 @@
     <t xml:space="preserve">Resource Language (field_doc_language) </t>
   </si>
   <si>
-    <t>Check process (only values from the list of Resource type). TODO: Use iso code. Remove this taxonomy and use Drupal Lang ?</t>
-  </si>
-  <si>
     <t>Author(s)</t>
   </si>
   <si>
@@ -117,15 +111,9 @@
     <t>Link to the publication</t>
   </si>
   <si>
-    <t>Link field with a static "adhoc" title for all: "Click here to access the resource"</t>
-  </si>
-  <si>
     <t xml:space="preserve">Copyright (field_doc_copyrights_statement) </t>
   </si>
   <si>
-    <t>Think to udpdate/remove this field</t>
-  </si>
-  <si>
     <t>Thumbnail</t>
   </si>
   <si>
@@ -150,9 +138,6 @@
     <t xml:space="preserve">Data Provider (Entity reference by Entity label) (field_doc_provider:label) </t>
   </si>
   <si>
-    <t xml:space="preserve"> Long text. One author per line (uses some php code)</t>
-  </si>
-  <si>
     <t>Process (PHP)</t>
   </si>
   <si>
@@ -168,9 +153,6 @@
     <t>Process (more than one value)</t>
   </si>
   <si>
-    <t>Check process (only values from the list of Resource type).  "," values separator</t>
-  </si>
-  <si>
     <t>Overarching Categories (field_related_domains)</t>
   </si>
   <si>
@@ -189,9 +171,6 @@
     <t xml:space="preserve">Related Concepts (field_related_topics) </t>
   </si>
   <si>
-    <t>The value of the field must match the region label. "," values separator (as far as concepts has not commas (','))</t>
-  </si>
-  <si>
     <t xml:space="preserve">Geographical focus (field_geographical_focus) </t>
   </si>
   <si>
@@ -222,10 +201,43 @@
     <t>Themes</t>
   </si>
   <si>
-    <t>Copyright owner</t>
-  </si>
-  <si>
     <t>The value of the field must match the organization label.  ";" values separator</t>
+  </si>
+  <si>
+    <t>Check process (only values from the list of Resource type).  ";" values separator</t>
+  </si>
+  <si>
+    <t>Long text. One author per line (uses some php code)</t>
+  </si>
+  <si>
+    <t>The value of the field must match the region label. ";" values separator (as far as concepts has not commas (','))</t>
+  </si>
+  <si>
+    <t>Copyright details</t>
+  </si>
+  <si>
+    <t>Pages</t>
+  </si>
+  <si>
+    <t>Pages (field_doc_pagination)</t>
+  </si>
+  <si>
+    <t>License</t>
+  </si>
+  <si>
+    <t xml:space="preserve">License (field_doc_licencing) </t>
+  </si>
+  <si>
+    <t>Link to the original website</t>
+  </si>
+  <si>
+    <t>Published at: URL (field_doc_is_shown_at:url)</t>
+  </si>
+  <si>
+    <t>Link field with a static "adhoc" title for all: "Access original publishing page"</t>
+  </si>
+  <si>
+    <t>Link field with a static "adhoc" title for all: "Download the resource"</t>
   </si>
 </sst>
 </file>
@@ -1069,10 +1081,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1085,23 +1097,23 @@
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>2</v>
@@ -1112,151 +1124,151 @@
     </row>
     <row r="4" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>3</v>
+        <v>43</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>21</v>
-      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="6"/>
+      <c r="A9" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="10" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D10" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="10"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="10"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
+      <c r="D12" s="4" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="13" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="1" t="s">
+      <c r="A14" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="6"/>
+    </row>
+    <row r="15" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="6"/>
     </row>
     <row r="16" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>1</v>
@@ -1267,156 +1279,180 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="12" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C22" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>32</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>36</v>
+        <v>72</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="9" t="s">
-        <v>29</v>
+      <c r="A27" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B28" s="1" t="s">
+      <c r="A28" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D28" s="4" t="s">
-        <v>34</v>
-      </c>
+      <c r="D29" s="4"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="C31" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="D31" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D30" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C32" t="s">
-        <v>60</v>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C33" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>